<commit_message>
updates Fig 4 with data v5
</commit_message>
<xml_diff>
--- a/rawdata/supplementary_material_V5.xlsx
+++ b/rawdata/supplementary_material_V5.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20376"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D62E0B6-0D73-407E-817B-6A0FD2B31E06}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B1AB6A8-0119-4DF8-A7A9-6CCE0B52577A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" tabRatio="859" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" tabRatio="859" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scoring system" sheetId="1" r:id="rId1"/>
@@ -5320,9 +5320,6 @@
 (5) Fight Illegal, Unreported and Unregulated (IUU) fishing.</t>
   </si>
   <si>
-    <t>Les AMP sont en partie créées pour préserver le patrimoine culturel et naturel.The Great Bear Sea and the Gwaii Haanas National Marine Conservation Area Reserve and Haida Heritage Site in BC, Canada serves as a good example</t>
-  </si>
-  <si>
     <t>Sustainable fishing practices included the reduction of wastes comming from gear loss. Fishing activities make substantial contribution to the amount of marine detritus in the ocean. Some debris such as fishing gears are found on the deep seafloor.</t>
   </si>
   <si>
@@ -5796,6 +5793,9 @@
   <si>
     <t xml:space="preserve">The support to the developing countries to facilitate support to developing countries is provided through programs such as REDD+. Also, taking into account the potential of the different forests NCS to remove CO2, developing countries can strengthen their scientific and technological capacity to move towards more sustainable patterns of consumption and production using founds from the financial transfers from North to South under global carbon pricing. 
 However, the scientific capacity if developing countries can be undermined because science research can be associated with parachute science (western scientists briefly conducting field research in a developing country then completing the research in their home country). If local researcher are not included in monitoring programs and related research, negatively impact the scientific research in developing countries. </t>
+  </si>
+  <si>
+    <t>MPAs are created in part to preserve cultural and natural heritage. The Great Bear Sea and the Gwaii Haanas National Marine Conservation Area Reserve and Haida Heritage Site in BC, Canada serves as a good example</t>
   </si>
 </sst>
 </file>
@@ -6464,6 +6464,12 @@
     <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -6473,11 +6479,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -6485,19 +6491,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6510,9 +6510,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6528,6 +6525,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -6975,10 +6975,10 @@
       <c r="D3" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="125" t="s">
+      <c r="E3" s="123" t="s">
         <v>831</v>
       </c>
-      <c r="F3" s="125" t="s">
+      <c r="F3" s="123" t="s">
         <v>562</v>
       </c>
     </row>
@@ -6995,8 +6995,8 @@
       <c r="D4" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="125"/>
-      <c r="F4" s="125"/>
+      <c r="E4" s="123"/>
+      <c r="F4" s="123"/>
     </row>
     <row r="5" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
@@ -7121,10 +7121,10 @@
       <c r="D11" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="125" t="s">
+      <c r="E11" s="123" t="s">
         <v>568</v>
       </c>
-      <c r="F11" s="125" t="s">
+      <c r="F11" s="123" t="s">
         <v>569</v>
       </c>
     </row>
@@ -7141,8 +7141,8 @@
       <c r="D12" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="125"/>
-      <c r="F12" s="125"/>
+      <c r="E12" s="123"/>
+      <c r="F12" s="123"/>
     </row>
     <row r="13" spans="1:6" ht="232.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="22" t="s">
@@ -7157,8 +7157,8 @@
       <c r="D13" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="125"/>
-      <c r="F13" s="125"/>
+      <c r="E13" s="123"/>
+      <c r="F13" s="123"/>
     </row>
     <row r="14" spans="1:6" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A14" s="22" t="s">
@@ -7283,10 +7283,10 @@
       <c r="D20" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="125" t="s">
+      <c r="E20" s="123" t="s">
         <v>977</v>
       </c>
-      <c r="F20" s="125" t="s">
+      <c r="F20" s="123" t="s">
         <v>976</v>
       </c>
     </row>
@@ -7303,8 +7303,8 @@
       <c r="D21" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="125"/>
-      <c r="F21" s="125"/>
+      <c r="E21" s="123"/>
+      <c r="F21" s="123"/>
     </row>
     <row r="22" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A22" s="22" t="s">
@@ -7610,10 +7610,10 @@
         <v>8</v>
       </c>
       <c r="E37" s="31" t="s">
+        <v>1074</v>
+      </c>
+      <c r="F37" s="31" t="s">
         <v>1075</v>
-      </c>
-      <c r="F37" s="31" t="s">
-        <v>1076</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
@@ -7673,7 +7673,7 @@
         <v>998</v>
       </c>
       <c r="F40" s="39" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
@@ -8229,10 +8229,10 @@
       <c r="D70" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="E70" s="125" t="s">
+      <c r="E70" s="123" t="s">
         <v>982</v>
       </c>
-      <c r="F70" s="125" t="s">
+      <c r="F70" s="123" t="s">
         <v>983</v>
       </c>
     </row>
@@ -8249,8 +8249,8 @@
       <c r="D71" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="E71" s="125"/>
-      <c r="F71" s="125"/>
+      <c r="E71" s="123"/>
+      <c r="F71" s="123"/>
     </row>
     <row r="72" spans="1:6" ht="78" x14ac:dyDescent="0.3">
       <c r="A72" s="22" t="s">
@@ -8535,10 +8535,10 @@
       <c r="D86" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="E86" s="118" t="s">
+      <c r="E86" s="120" t="s">
         <v>1000</v>
       </c>
-      <c r="F86" s="118" t="s">
+      <c r="F86" s="120" t="s">
         <v>1001</v>
       </c>
     </row>
@@ -8555,8 +8555,8 @@
       <c r="D87" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="E87" s="118"/>
-      <c r="F87" s="118"/>
+      <c r="E87" s="120"/>
+      <c r="F87" s="120"/>
     </row>
     <row r="88" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="22" t="s">
@@ -8571,8 +8571,8 @@
       <c r="D88" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="E88" s="118"/>
-      <c r="F88" s="118"/>
+      <c r="E88" s="120"/>
+      <c r="F88" s="120"/>
     </row>
     <row r="89" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A89" s="22" t="s">
@@ -8658,7 +8658,7 @@
         <v>8</v>
       </c>
       <c r="E93" s="31" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="F93" s="31" t="s">
         <v>29</v>
@@ -8908,7 +8908,7 @@
         <v>6</v>
       </c>
       <c r="E106" s="113" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="F106" s="31" t="s">
         <v>29</v>
@@ -9057,10 +9057,10 @@
       <c r="D114" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="E114" s="125" t="s">
+      <c r="E114" s="123" t="s">
         <v>581</v>
       </c>
-      <c r="F114" s="125" t="s">
+      <c r="F114" s="123" t="s">
         <v>290</v>
       </c>
     </row>
@@ -9077,8 +9077,8 @@
       <c r="D115" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="E115" s="125"/>
-      <c r="F115" s="125"/>
+      <c r="E115" s="123"/>
+      <c r="F115" s="123"/>
     </row>
     <row r="116" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A116" s="22" t="s">
@@ -9113,10 +9113,10 @@
       <c r="D117" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="E117" s="123" t="s">
-        <v>1005</v>
-      </c>
-      <c r="F117" s="123" t="s">
+      <c r="E117" s="125" t="s">
+        <v>1004</v>
+      </c>
+      <c r="F117" s="125" t="s">
         <v>586</v>
       </c>
     </row>
@@ -9133,8 +9133,8 @@
       <c r="D118" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="E118" s="124"/>
-      <c r="F118" s="124"/>
+      <c r="E118" s="126"/>
+      <c r="F118" s="126"/>
     </row>
     <row r="119" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A119" s="22" t="s">
@@ -9208,10 +9208,10 @@
         <v>8</v>
       </c>
       <c r="E122" s="31" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="F122" s="31" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="123" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
@@ -9837,11 +9837,11 @@
       <c r="D156" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="E156" s="125" t="s">
+      <c r="E156" s="123" t="s">
+        <v>1005</v>
+      </c>
+      <c r="F156" s="123" t="s">
         <v>1006</v>
-      </c>
-      <c r="F156" s="125" t="s">
-        <v>1007</v>
       </c>
     </row>
     <row r="157" spans="1:6" ht="163.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -9857,8 +9857,8 @@
       <c r="D157" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="E157" s="125"/>
-      <c r="F157" s="125"/>
+      <c r="E157" s="123"/>
+      <c r="F157" s="123"/>
     </row>
     <row r="158" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A158" s="22" t="s">
@@ -9954,7 +9954,7 @@
         <v>8</v>
       </c>
       <c r="E162" s="39" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="F162" s="39" t="s">
         <v>170</v>
@@ -10034,10 +10034,10 @@
         <v>8</v>
       </c>
       <c r="E166" s="31" t="s">
+        <v>1008</v>
+      </c>
+      <c r="F166" s="31" t="s">
         <v>1009</v>
-      </c>
-      <c r="F166" s="31" t="s">
-        <v>1010</v>
       </c>
     </row>
     <row r="167" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
@@ -10062,6 +10062,25 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="E86:E88"/>
+    <mergeCell ref="F86:F88"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A44:F44"/>
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="A63:F63"/>
+    <mergeCell ref="A69:F69"/>
+    <mergeCell ref="E70:E71"/>
+    <mergeCell ref="F70:F71"/>
+    <mergeCell ref="A82:F82"/>
     <mergeCell ref="E156:E157"/>
     <mergeCell ref="F156:F157"/>
     <mergeCell ref="A91:F91"/>
@@ -10077,25 +10096,6 @@
     <mergeCell ref="A155:F155"/>
     <mergeCell ref="E117:E118"/>
     <mergeCell ref="F117:F118"/>
-    <mergeCell ref="E86:E88"/>
-    <mergeCell ref="F86:F88"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A44:F44"/>
-    <mergeCell ref="A54:F54"/>
-    <mergeCell ref="A63:F63"/>
-    <mergeCell ref="A69:F69"/>
-    <mergeCell ref="E70:E71"/>
-    <mergeCell ref="F70:F71"/>
-    <mergeCell ref="A82:F82"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="F11:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -11548,10 +11548,10 @@
       <c r="D76" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="E76" s="123" t="s">
+      <c r="E76" s="125" t="s">
         <v>610</v>
       </c>
-      <c r="F76" s="123" t="s">
+      <c r="F76" s="125" t="s">
         <v>611</v>
       </c>
     </row>
@@ -11568,8 +11568,8 @@
       <c r="D77" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="E77" s="124"/>
-      <c r="F77" s="124"/>
+      <c r="E77" s="126"/>
+      <c r="F77" s="126"/>
     </row>
     <row r="78" spans="1:6" ht="195" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="22" t="s">
@@ -11755,10 +11755,10 @@
         <v>8</v>
       </c>
       <c r="E87" s="95" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="F87" s="31" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="78" x14ac:dyDescent="0.3">
@@ -11905,7 +11905,7 @@
         <v>6</v>
       </c>
       <c r="E95" s="113" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="F95" s="113" t="s">
         <v>29</v>
@@ -13281,14 +13281,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A142:F142"/>
-    <mergeCell ref="A155:F155"/>
-    <mergeCell ref="A102:F102"/>
-    <mergeCell ref="A113:F113"/>
-    <mergeCell ref="A125:F125"/>
-    <mergeCell ref="E126:E127"/>
-    <mergeCell ref="F126:F127"/>
-    <mergeCell ref="A131:F131"/>
     <mergeCell ref="A91:F91"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A10:F10"/>
@@ -13301,6 +13293,14 @@
     <mergeCell ref="A82:F82"/>
     <mergeCell ref="E76:E77"/>
     <mergeCell ref="F76:F77"/>
+    <mergeCell ref="A142:F142"/>
+    <mergeCell ref="A155:F155"/>
+    <mergeCell ref="A102:F102"/>
+    <mergeCell ref="A113:F113"/>
+    <mergeCell ref="A125:F125"/>
+    <mergeCell ref="E126:E127"/>
+    <mergeCell ref="F126:F127"/>
+    <mergeCell ref="A131:F131"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -13514,10 +13514,10 @@
       <c r="D11" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="123" t="s">
+      <c r="E11" s="125" t="s">
         <v>635</v>
       </c>
-      <c r="F11" s="123" t="s">
+      <c r="F11" s="125" t="s">
         <v>841</v>
       </c>
     </row>
@@ -13534,8 +13534,8 @@
       <c r="D12" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="124"/>
-      <c r="F12" s="124"/>
+      <c r="E12" s="126"/>
+      <c r="F12" s="126"/>
     </row>
     <row r="13" spans="1:6" ht="114" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="22" t="s">
@@ -13678,10 +13678,10 @@
       <c r="D20" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="123" t="s">
+      <c r="E20" s="125" t="s">
         <v>636</v>
       </c>
-      <c r="F20" s="123" t="s">
+      <c r="F20" s="125" t="s">
         <v>637</v>
       </c>
     </row>
@@ -13698,8 +13698,8 @@
       <c r="D21" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="124"/>
-      <c r="F21" s="124"/>
+      <c r="E21" s="126"/>
+      <c r="F21" s="126"/>
     </row>
     <row r="22" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A22" s="22" t="s">
@@ -14624,10 +14624,10 @@
       <c r="D70" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="E70" s="123" t="s">
+      <c r="E70" s="125" t="s">
         <v>644</v>
       </c>
-      <c r="F70" s="123" t="s">
+      <c r="F70" s="125" t="s">
         <v>645</v>
       </c>
     </row>
@@ -14644,8 +14644,8 @@
       <c r="D71" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="E71" s="124"/>
-      <c r="F71" s="124"/>
+      <c r="E71" s="126"/>
+      <c r="F71" s="126"/>
     </row>
     <row r="72" spans="1:6" ht="78" x14ac:dyDescent="0.3">
       <c r="A72" s="22" t="s">
@@ -14951,10 +14951,10 @@
         <v>8</v>
       </c>
       <c r="E87" s="65" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="F87" s="65" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="78" x14ac:dyDescent="0.3">
@@ -15101,7 +15101,7 @@
         <v>6</v>
       </c>
       <c r="E95" s="113" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="F95" s="113" t="s">
         <v>29</v>
@@ -15850,10 +15850,10 @@
       <c r="D135" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="E135" s="123" t="s">
+      <c r="E135" s="125" t="s">
         <v>653</v>
       </c>
-      <c r="F135" s="123" t="s">
+      <c r="F135" s="125" t="s">
         <v>646</v>
       </c>
     </row>
@@ -15870,8 +15870,8 @@
       <c r="D136" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="E136" s="124"/>
-      <c r="F136" s="124"/>
+      <c r="E136" s="126"/>
+      <c r="F136" s="126"/>
     </row>
     <row r="137" spans="1:6" ht="124.8" x14ac:dyDescent="0.3">
       <c r="A137" s="22" t="s">
@@ -16480,13 +16480,11 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="A131:F131"/>
+    <mergeCell ref="E135:E136"/>
+    <mergeCell ref="F135:F136"/>
+    <mergeCell ref="A142:F142"/>
+    <mergeCell ref="A155:F155"/>
     <mergeCell ref="E126:E127"/>
     <mergeCell ref="F126:F127"/>
     <mergeCell ref="A33:F33"/>
@@ -16501,11 +16499,13 @@
     <mergeCell ref="A102:F102"/>
     <mergeCell ref="A113:F113"/>
     <mergeCell ref="A125:F125"/>
-    <mergeCell ref="A131:F131"/>
-    <mergeCell ref="E135:E136"/>
-    <mergeCell ref="F135:F136"/>
-    <mergeCell ref="A142:F142"/>
-    <mergeCell ref="A155:F155"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="A19:F19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16515,8 +16515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:F167"/>
   <sheetViews>
-    <sheetView topLeftCell="A120" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F122" sqref="F122"/>
+    <sheetView tabSelected="1" topLeftCell="A102" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E107" sqref="E107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16547,14 +16547,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="121" t="s">
+      <c r="A2" s="118" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="122"/>
-      <c r="C2" s="122"/>
-      <c r="D2" s="122"/>
-      <c r="E2" s="122"/>
-      <c r="F2" s="122"/>
+      <c r="B2" s="119"/>
+      <c r="C2" s="119"/>
+      <c r="D2" s="119"/>
+      <c r="E2" s="119"/>
+      <c r="F2" s="119"/>
     </row>
     <row r="3" spans="1:6" ht="67.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
@@ -16569,10 +16569,10 @@
       <c r="D3" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="123" t="s">
+      <c r="E3" s="125" t="s">
         <v>939</v>
       </c>
-      <c r="F3" s="123" t="s">
+      <c r="F3" s="125" t="s">
         <v>940</v>
       </c>
     </row>
@@ -16589,8 +16589,8 @@
       <c r="D4" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="124"/>
-      <c r="F4" s="124"/>
+      <c r="E4" s="126"/>
+      <c r="F4" s="126"/>
     </row>
     <row r="5" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
@@ -16642,10 +16642,10 @@
         <v>8</v>
       </c>
       <c r="E7" s="107" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="F7" s="107" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="93.6" x14ac:dyDescent="0.3">
@@ -16661,11 +16661,11 @@
       <c r="D8" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="123" t="s">
+      <c r="E8" s="125" t="s">
+        <v>1033</v>
+      </c>
+      <c r="F8" s="125" t="s">
         <v>1034</v>
-      </c>
-      <c r="F8" s="123" t="s">
-        <v>1035</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
@@ -16681,8 +16681,8 @@
       <c r="D9" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="124"/>
-      <c r="F9" s="124"/>
+      <c r="E9" s="126"/>
+      <c r="F9" s="126"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="117" t="s">
@@ -16708,10 +16708,10 @@
         <v>8</v>
       </c>
       <c r="E11" s="133" t="s">
-        <v>1088</v>
-      </c>
-      <c r="F11" s="119" t="s">
         <v>1087</v>
+      </c>
+      <c r="F11" s="121" t="s">
+        <v>1086</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="78" x14ac:dyDescent="0.3">
@@ -16727,7 +16727,7 @@
       <c r="D12" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="134"/>
+      <c r="E12" s="139"/>
       <c r="F12" s="130"/>
     </row>
     <row r="13" spans="1:6" ht="135.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -16743,8 +16743,8 @@
       <c r="D13" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="135"/>
-      <c r="F13" s="120"/>
+      <c r="E13" s="134"/>
+      <c r="F13" s="122"/>
     </row>
     <row r="14" spans="1:6" ht="234" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="22" t="s">
@@ -16760,10 +16760,10 @@
         <v>6</v>
       </c>
       <c r="E14" s="107" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="F14" s="107" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="109.2" x14ac:dyDescent="0.3">
@@ -16869,10 +16869,10 @@
       <c r="D20" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="119" t="s">
+      <c r="E20" s="121" t="s">
         <v>943</v>
       </c>
-      <c r="F20" s="119" t="s">
+      <c r="F20" s="121" t="s">
         <v>923</v>
       </c>
     </row>
@@ -16889,8 +16889,8 @@
       <c r="D21" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="120"/>
-      <c r="F21" s="120"/>
+      <c r="E21" s="122"/>
+      <c r="F21" s="122"/>
     </row>
     <row r="22" spans="1:6" ht="46.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="22" t="s">
@@ -17192,10 +17192,10 @@
         <v>8</v>
       </c>
       <c r="E37" s="114" t="s">
+        <v>1074</v>
+      </c>
+      <c r="F37" s="107" t="s">
         <v>1075</v>
-      </c>
-      <c r="F37" s="107" t="s">
-        <v>1076</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
@@ -17255,7 +17255,7 @@
         <v>999</v>
       </c>
       <c r="F40" s="107" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
@@ -17342,10 +17342,10 @@
         <v>8</v>
       </c>
       <c r="E45" s="113" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="F45" s="113" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
@@ -17701,10 +17701,10 @@
       <c r="D64" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="E64" s="136" t="s">
+      <c r="E64" s="135" t="s">
         <v>949</v>
       </c>
-      <c r="F64" s="123" t="s">
+      <c r="F64" s="125" t="s">
         <v>950</v>
       </c>
     </row>
@@ -17721,8 +17721,8 @@
       <c r="D65" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="E65" s="137"/>
-      <c r="F65" s="124"/>
+      <c r="E65" s="136"/>
+      <c r="F65" s="126"/>
     </row>
     <row r="66" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A66" s="22" t="s">
@@ -17807,10 +17807,10 @@
       <c r="D70" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="E70" s="123" t="s">
+      <c r="E70" s="125" t="s">
         <v>951</v>
       </c>
-      <c r="F70" s="123" t="s">
+      <c r="F70" s="125" t="s">
         <v>951</v>
       </c>
     </row>
@@ -17827,8 +17827,8 @@
       <c r="D71" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="E71" s="124"/>
-      <c r="F71" s="124"/>
+      <c r="E71" s="126"/>
+      <c r="F71" s="126"/>
     </row>
     <row r="72" spans="1:6" ht="78" x14ac:dyDescent="0.3">
       <c r="A72" s="22" t="s">
@@ -17915,10 +17915,10 @@
       <c r="D76" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="E76" s="138" t="s">
+      <c r="E76" s="137" t="s">
         <v>955</v>
       </c>
-      <c r="F76" s="123" t="s">
+      <c r="F76" s="125" t="s">
         <v>956</v>
       </c>
     </row>
@@ -17935,8 +17935,8 @@
       <c r="D77" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="E77" s="139"/>
-      <c r="F77" s="124"/>
+      <c r="E77" s="138"/>
+      <c r="F77" s="126"/>
     </row>
     <row r="78" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A78" s="22" t="s">
@@ -18087,11 +18087,11 @@
       <c r="D86" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="E86" s="129" t="s">
-        <v>1053</v>
-      </c>
-      <c r="F86" s="118" t="s">
-        <v>1059</v>
+      <c r="E86" s="128" t="s">
+        <v>1052</v>
+      </c>
+      <c r="F86" s="120" t="s">
+        <v>1058</v>
       </c>
     </row>
     <row r="87" spans="1:6" ht="93.6" x14ac:dyDescent="0.3">
@@ -18107,8 +18107,8 @@
       <c r="D87" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="E87" s="129"/>
-      <c r="F87" s="118"/>
+      <c r="E87" s="128"/>
+      <c r="F87" s="120"/>
     </row>
     <row r="88" spans="1:6" ht="158.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="22" t="s">
@@ -18123,8 +18123,8 @@
       <c r="D88" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="E88" s="129"/>
-      <c r="F88" s="118"/>
+      <c r="E88" s="128"/>
+      <c r="F88" s="120"/>
     </row>
     <row r="89" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A89" s="22" t="s">
@@ -18250,7 +18250,7 @@
         <v>6</v>
       </c>
       <c r="E95" s="113" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="F95" s="113" t="s">
         <v>29</v>
@@ -18290,10 +18290,10 @@
         <v>8</v>
       </c>
       <c r="E97" s="43" t="s">
+        <v>1011</v>
+      </c>
+      <c r="F97" s="107" t="s">
         <v>1012</v>
-      </c>
-      <c r="F97" s="107" t="s">
-        <v>1013</v>
       </c>
     </row>
     <row r="98" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
@@ -18350,7 +18350,7 @@
         <v>8</v>
       </c>
       <c r="E100" s="43" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="F100" s="107" t="s">
         <v>918</v>
@@ -18460,7 +18460,7 @@
         <v>6</v>
       </c>
       <c r="E106" s="43" t="s">
-        <v>1004</v>
+        <v>1110</v>
       </c>
       <c r="F106" s="107" t="s">
         <v>29</v>
@@ -18609,10 +18609,10 @@
       <c r="D114" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="E114" s="125" t="s">
+      <c r="E114" s="123" t="s">
         <v>958</v>
       </c>
-      <c r="F114" s="125" t="s">
+      <c r="F114" s="123" t="s">
         <v>290</v>
       </c>
     </row>
@@ -18629,8 +18629,8 @@
       <c r="D115" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="E115" s="125"/>
-      <c r="F115" s="125"/>
+      <c r="E115" s="123"/>
+      <c r="F115" s="123"/>
     </row>
     <row r="116" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A116" s="22" t="s">
@@ -18665,10 +18665,10 @@
       <c r="D117" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="E117" s="123" t="s">
-        <v>1005</v>
-      </c>
-      <c r="F117" s="123" t="s">
+      <c r="E117" s="125" t="s">
+        <v>1004</v>
+      </c>
+      <c r="F117" s="125" t="s">
         <v>586</v>
       </c>
     </row>
@@ -18685,8 +18685,8 @@
       <c r="D118" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="E118" s="124"/>
-      <c r="F118" s="124"/>
+      <c r="E118" s="126"/>
+      <c r="F118" s="126"/>
     </row>
     <row r="119" spans="1:6" ht="127.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="22" t="s">
@@ -18760,10 +18760,10 @@
         <v>8</v>
       </c>
       <c r="E122" s="43" t="s">
+        <v>1101</v>
+      </c>
+      <c r="F122" s="107" t="s">
         <v>1102</v>
-      </c>
-      <c r="F122" s="107" t="s">
-        <v>1103</v>
       </c>
     </row>
     <row r="123" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
@@ -18829,10 +18829,10 @@
       <c r="D126" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="E126" s="119" t="s">
+      <c r="E126" s="121" t="s">
         <v>962</v>
       </c>
-      <c r="F126" s="119" t="s">
+      <c r="F126" s="121" t="s">
         <v>916</v>
       </c>
     </row>
@@ -18865,8 +18865,8 @@
       <c r="D128" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="E128" s="120"/>
-      <c r="F128" s="120"/>
+      <c r="E128" s="122"/>
+      <c r="F128" s="122"/>
     </row>
     <row r="129" spans="1:6" ht="109.2" x14ac:dyDescent="0.3">
       <c r="A129" s="22" t="s">
@@ -18951,8 +18951,8 @@
       <c r="D133" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="E133" s="135"/>
-      <c r="F133" s="135"/>
+      <c r="E133" s="134"/>
+      <c r="F133" s="134"/>
     </row>
     <row r="134" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A134" s="22" t="s">
@@ -19246,10 +19246,10 @@
         <v>8</v>
       </c>
       <c r="E149" s="43" t="s">
+        <v>1092</v>
+      </c>
+      <c r="F149" s="115" t="s">
         <v>1093</v>
-      </c>
-      <c r="F149" s="115" t="s">
-        <v>1094</v>
       </c>
     </row>
     <row r="150" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
@@ -19346,10 +19346,10 @@
         <v>8</v>
       </c>
       <c r="E154" s="43" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="F154" s="107" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.3">
@@ -19375,11 +19375,11 @@
       <c r="D156" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="E156" s="119" t="s">
-        <v>1065</v>
-      </c>
-      <c r="F156" s="123" t="s">
-        <v>1008</v>
+      <c r="E156" s="121" t="s">
+        <v>1064</v>
+      </c>
+      <c r="F156" s="125" t="s">
+        <v>1007</v>
       </c>
     </row>
     <row r="157" spans="1:6" ht="162" customHeight="1" x14ac:dyDescent="0.3">
@@ -19395,8 +19395,8 @@
       <c r="D157" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="E157" s="120"/>
-      <c r="F157" s="124"/>
+      <c r="E157" s="122"/>
+      <c r="F157" s="126"/>
     </row>
     <row r="158" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A158" s="22" t="s">
@@ -19411,10 +19411,10 @@
       <c r="D158" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="E158" s="119" t="s">
+      <c r="E158" s="121" t="s">
         <v>966</v>
       </c>
-      <c r="F158" s="123" t="s">
+      <c r="F158" s="125" t="s">
         <v>967</v>
       </c>
     </row>
@@ -19431,8 +19431,8 @@
       <c r="D159" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="E159" s="120"/>
-      <c r="F159" s="124"/>
+      <c r="E159" s="122"/>
+      <c r="F159" s="126"/>
     </row>
     <row r="160" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A160" s="22" t="s">
@@ -19480,7 +19480,7 @@
         <v>8</v>
       </c>
       <c r="E162" s="106" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="F162" s="106" t="s">
         <v>170</v>
@@ -19548,10 +19548,10 @@
         <v>8</v>
       </c>
       <c r="E166" s="112" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="F166" s="112" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="167" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
@@ -19572,6 +19572,34 @@
     </row>
   </sheetData>
   <mergeCells count="44">
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A44:F44"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="F114:F115"/>
+    <mergeCell ref="A113:F113"/>
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="A63:F63"/>
+    <mergeCell ref="A69:F69"/>
+    <mergeCell ref="A82:F82"/>
+    <mergeCell ref="A91:F91"/>
+    <mergeCell ref="A102:F102"/>
+    <mergeCell ref="E64:E65"/>
+    <mergeCell ref="F64:F65"/>
+    <mergeCell ref="E76:E77"/>
+    <mergeCell ref="F76:F77"/>
+    <mergeCell ref="E86:E88"/>
+    <mergeCell ref="F86:F88"/>
+    <mergeCell ref="E70:E71"/>
     <mergeCell ref="F70:F71"/>
     <mergeCell ref="E117:E118"/>
     <mergeCell ref="F117:F118"/>
@@ -19588,34 +19616,6 @@
     <mergeCell ref="A131:F131"/>
     <mergeCell ref="A142:F142"/>
     <mergeCell ref="E114:E115"/>
-    <mergeCell ref="F114:F115"/>
-    <mergeCell ref="A113:F113"/>
-    <mergeCell ref="A54:F54"/>
-    <mergeCell ref="A63:F63"/>
-    <mergeCell ref="A69:F69"/>
-    <mergeCell ref="A82:F82"/>
-    <mergeCell ref="A91:F91"/>
-    <mergeCell ref="A102:F102"/>
-    <mergeCell ref="E64:E65"/>
-    <mergeCell ref="F64:F65"/>
-    <mergeCell ref="E76:E77"/>
-    <mergeCell ref="F76:F77"/>
-    <mergeCell ref="E86:E88"/>
-    <mergeCell ref="F86:F88"/>
-    <mergeCell ref="E70:E71"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A44:F44"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="F11:F13"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -19659,14 +19659,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="121" t="s">
+      <c r="A2" s="118" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="122"/>
-      <c r="C2" s="122"/>
-      <c r="D2" s="122"/>
-      <c r="E2" s="122"/>
-      <c r="F2" s="122"/>
+      <c r="B2" s="119"/>
+      <c r="C2" s="119"/>
+      <c r="D2" s="119"/>
+      <c r="E2" s="119"/>
+      <c r="F2" s="119"/>
     </row>
     <row r="3" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
@@ -20812,7 +20812,7 @@
         <v>8</v>
       </c>
       <c r="E62" s="29" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="F62" s="29" t="s">
         <v>170</v>
@@ -21282,10 +21282,10 @@
         <v>8</v>
       </c>
       <c r="E87" s="27" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="F87" s="27" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="78" x14ac:dyDescent="0.3">
@@ -22019,10 +22019,10 @@
       <c r="D126" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="E126" s="118" t="s">
+      <c r="E126" s="120" t="s">
         <v>433</v>
       </c>
-      <c r="F126" s="119" t="s">
+      <c r="F126" s="121" t="s">
         <v>434</v>
       </c>
     </row>
@@ -22039,8 +22039,8 @@
       <c r="D127" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="E127" s="118"/>
-      <c r="F127" s="120"/>
+      <c r="E127" s="120"/>
+      <c r="F127" s="122"/>
     </row>
     <row r="128" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A128" s="22" t="s">
@@ -22706,7 +22706,7 @@
         <v>8</v>
       </c>
       <c r="E162" s="52" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="F162" s="29" t="s">
         <v>170</v>
@@ -22814,12 +22814,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A54:F54"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A44:F44"/>
     <mergeCell ref="A155:F155"/>
     <mergeCell ref="A63:F63"/>
     <mergeCell ref="A69:F69"/>
@@ -22832,6 +22826,12 @@
     <mergeCell ref="F126:F127"/>
     <mergeCell ref="A131:F131"/>
     <mergeCell ref="A142:F142"/>
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A44:F44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -22895,10 +22895,10 @@
       <c r="D3" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="118" t="s">
+      <c r="E3" s="120" t="s">
         <v>828</v>
       </c>
-      <c r="F3" s="118" t="s">
+      <c r="F3" s="120" t="s">
         <v>829</v>
       </c>
     </row>
@@ -22915,8 +22915,8 @@
       <c r="D4" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="118"/>
-      <c r="F4" s="118"/>
+      <c r="E4" s="120"/>
+      <c r="F4" s="120"/>
     </row>
     <row r="5" spans="1:6" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
@@ -22972,10 +22972,10 @@
         <v>8</v>
       </c>
       <c r="E7" s="27" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="F7" s="27" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="271.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -23012,10 +23012,10 @@
         <v>8</v>
       </c>
       <c r="E9" s="27" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="F9" s="27" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -23041,10 +23041,10 @@
       <c r="D11" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="123" t="s">
-        <v>1085</v>
-      </c>
-      <c r="F11" s="125" t="s">
+      <c r="E11" s="125" t="s">
+        <v>1084</v>
+      </c>
+      <c r="F11" s="123" t="s">
         <v>837</v>
       </c>
     </row>
@@ -23061,8 +23061,8 @@
       <c r="D12" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="126"/>
-      <c r="F12" s="126"/>
+      <c r="E12" s="127"/>
+      <c r="F12" s="127"/>
     </row>
     <row r="13" spans="1:6" ht="130.94999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="22" t="s">
@@ -23077,8 +23077,8 @@
       <c r="D13" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="124"/>
-      <c r="F13" s="124"/>
+      <c r="E13" s="126"/>
+      <c r="F13" s="126"/>
     </row>
     <row r="14" spans="1:6" ht="228.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="22" t="s">
@@ -23586,10 +23586,10 @@
         <v>8</v>
       </c>
       <c r="E40" s="27" t="s">
+        <v>1089</v>
+      </c>
+      <c r="F40" s="27" t="s">
         <v>1090</v>
-      </c>
-      <c r="F40" s="27" t="s">
-        <v>1091</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
@@ -24006,7 +24006,7 @@
         <v>8</v>
       </c>
       <c r="E62" s="29" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="F62" s="29" t="s">
         <v>170</v>
@@ -24145,10 +24145,10 @@
       <c r="D70" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E70" s="118" t="s">
+      <c r="E70" s="120" t="s">
         <v>185</v>
       </c>
-      <c r="F70" s="118" t="s">
+      <c r="F70" s="120" t="s">
         <v>186</v>
       </c>
     </row>
@@ -24165,8 +24165,8 @@
       <c r="D71" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E71" s="118"/>
-      <c r="F71" s="118"/>
+      <c r="E71" s="120"/>
+      <c r="F71" s="120"/>
     </row>
     <row r="72" spans="1:6" ht="88.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="22" t="s">
@@ -24472,10 +24472,10 @@
         <v>8</v>
       </c>
       <c r="E87" s="27" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="F87" s="113" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="116.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -24981,10 +24981,10 @@
       <c r="D114" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="E114" s="125" t="s">
+      <c r="E114" s="123" t="s">
         <v>289</v>
       </c>
-      <c r="F114" s="125" t="s">
+      <c r="F114" s="123" t="s">
         <v>290</v>
       </c>
     </row>
@@ -25001,8 +25001,8 @@
       <c r="D115" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="E115" s="125"/>
-      <c r="F115" s="125"/>
+      <c r="E115" s="123"/>
+      <c r="F115" s="123"/>
     </row>
     <row r="116" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A116" s="22" t="s">
@@ -25138,10 +25138,10 @@
         <v>8</v>
       </c>
       <c r="E122" s="29" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="F122" s="36" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="123" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
@@ -25207,10 +25207,10 @@
       <c r="D126" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="E126" s="125" t="s">
+      <c r="E126" s="123" t="s">
         <v>315</v>
       </c>
-      <c r="F126" s="125" t="s">
+      <c r="F126" s="123" t="s">
         <v>316</v>
       </c>
     </row>
@@ -25227,8 +25227,8 @@
       <c r="D127" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="E127" s="125"/>
-      <c r="F127" s="125"/>
+      <c r="E127" s="123"/>
+      <c r="F127" s="123"/>
     </row>
     <row r="128" spans="1:6" ht="81" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="22" t="s">
@@ -25313,10 +25313,10 @@
       <c r="D132" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="E132" s="125" t="s">
+      <c r="E132" s="123" t="s">
         <v>328</v>
       </c>
-      <c r="F132" s="125" t="s">
+      <c r="F132" s="123" t="s">
         <v>329</v>
       </c>
     </row>
@@ -25333,8 +25333,8 @@
       <c r="D133" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="E133" s="125"/>
-      <c r="F133" s="125"/>
+      <c r="E133" s="123"/>
+      <c r="F133" s="123"/>
     </row>
     <row r="134" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A134" s="22" t="s">
@@ -25640,7 +25640,7 @@
         <v>8</v>
       </c>
       <c r="E149" s="29" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="F149" s="29" t="s">
         <v>366</v>
@@ -25699,10 +25699,10 @@
       <c r="D152" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="E152" s="127" t="s">
+      <c r="E152" s="124" t="s">
         <v>374</v>
       </c>
-      <c r="F152" s="127" t="s">
+      <c r="F152" s="124" t="s">
         <v>375</v>
       </c>
     </row>
@@ -25719,8 +25719,8 @@
       <c r="D153" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="E153" s="127"/>
-      <c r="F153" s="127"/>
+      <c r="E153" s="124"/>
+      <c r="F153" s="124"/>
     </row>
     <row r="154" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" s="22" t="s">
@@ -25736,7 +25736,7 @@
         <v>8</v>
       </c>
       <c r="E154" s="29" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="F154" s="29" t="s">
         <v>380</v>
@@ -25765,10 +25765,10 @@
       <c r="D156" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="E156" s="123" t="s">
-        <v>1097</v>
-      </c>
-      <c r="F156" s="123" t="s">
+      <c r="E156" s="125" t="s">
+        <v>1096</v>
+      </c>
+      <c r="F156" s="125" t="s">
         <v>384</v>
       </c>
     </row>
@@ -25785,8 +25785,8 @@
       <c r="D157" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="E157" s="124"/>
-      <c r="F157" s="124"/>
+      <c r="E157" s="126"/>
+      <c r="F157" s="126"/>
     </row>
     <row r="158" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A158" s="22" t="s">
@@ -25882,7 +25882,7 @@
         <v>8</v>
       </c>
       <c r="E162" s="29" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="F162" s="29" t="s">
         <v>170</v>
@@ -25962,10 +25962,10 @@
         <v>8</v>
       </c>
       <c r="E166" s="113" t="s">
+        <v>1068</v>
+      </c>
+      <c r="F166" s="112" t="s">
         <v>1069</v>
-      </c>
-      <c r="F166" s="112" t="s">
-        <v>1070</v>
       </c>
     </row>
     <row r="167" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
@@ -25990,22 +25990,6 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="A91:F91"/>
-    <mergeCell ref="A102:F102"/>
-    <mergeCell ref="A113:F113"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A44:F44"/>
-    <mergeCell ref="A54:F54"/>
-    <mergeCell ref="F70:F71"/>
-    <mergeCell ref="E70:E71"/>
-    <mergeCell ref="A63:F63"/>
-    <mergeCell ref="A69:F69"/>
-    <mergeCell ref="A82:F82"/>
-    <mergeCell ref="A131:F131"/>
-    <mergeCell ref="F114:F115"/>
-    <mergeCell ref="F132:F133"/>
-    <mergeCell ref="A142:F142"/>
-    <mergeCell ref="F152:F153"/>
     <mergeCell ref="A155:F155"/>
     <mergeCell ref="F156:F157"/>
     <mergeCell ref="E156:E157"/>
@@ -26022,6 +26006,22 @@
     <mergeCell ref="E126:E127"/>
     <mergeCell ref="A125:F125"/>
     <mergeCell ref="F126:F127"/>
+    <mergeCell ref="A131:F131"/>
+    <mergeCell ref="F114:F115"/>
+    <mergeCell ref="F132:F133"/>
+    <mergeCell ref="A142:F142"/>
+    <mergeCell ref="F152:F153"/>
+    <mergeCell ref="A91:F91"/>
+    <mergeCell ref="A102:F102"/>
+    <mergeCell ref="A113:F113"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A44:F44"/>
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="F70:F71"/>
+    <mergeCell ref="E70:E71"/>
+    <mergeCell ref="A63:F63"/>
+    <mergeCell ref="A69:F69"/>
+    <mergeCell ref="A82:F82"/>
   </mergeCells>
   <conditionalFormatting sqref="E109">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
@@ -26094,10 +26094,10 @@
       <c r="D3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="125" t="s">
+      <c r="E3" s="123" t="s">
         <v>830</v>
       </c>
-      <c r="F3" s="125" t="s">
+      <c r="F3" s="123" t="s">
         <v>445</v>
       </c>
     </row>
@@ -26114,8 +26114,8 @@
       <c r="D4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="125"/>
-      <c r="F4" s="125"/>
+      <c r="E4" s="123"/>
+      <c r="F4" s="123"/>
     </row>
     <row r="5" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
@@ -26240,10 +26240,10 @@
       <c r="D11" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="125" t="s">
+      <c r="E11" s="123" t="s">
         <v>449</v>
       </c>
-      <c r="F11" s="125" t="s">
+      <c r="F11" s="123" t="s">
         <v>450</v>
       </c>
     </row>
@@ -26260,8 +26260,8 @@
       <c r="D12" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="125"/>
-      <c r="F12" s="125"/>
+      <c r="E12" s="123"/>
+      <c r="F12" s="123"/>
     </row>
     <row r="13" spans="1:6" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A13" s="22" t="s">
@@ -26276,8 +26276,8 @@
       <c r="D13" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="125"/>
-      <c r="F13" s="125"/>
+      <c r="E13" s="123"/>
+      <c r="F13" s="123"/>
     </row>
     <row r="14" spans="1:6" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A14" s="22" t="s">
@@ -27212,7 +27212,7 @@
         <v>8</v>
       </c>
       <c r="E62" s="29" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="F62" s="29" t="s">
         <v>170</v>
@@ -27241,10 +27241,10 @@
       <c r="D64" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E64" s="125" t="s">
+      <c r="E64" s="123" t="s">
         <v>464</v>
       </c>
-      <c r="F64" s="125" t="s">
+      <c r="F64" s="123" t="s">
         <v>465</v>
       </c>
     </row>
@@ -27261,8 +27261,8 @@
       <c r="D65" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E65" s="125"/>
-      <c r="F65" s="125"/>
+      <c r="E65" s="123"/>
+      <c r="F65" s="123"/>
     </row>
     <row r="66" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A66" s="22" t="s">
@@ -27347,10 +27347,10 @@
       <c r="D70" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E70" s="125" t="s">
+      <c r="E70" s="123" t="s">
         <v>854</v>
       </c>
-      <c r="F70" s="125" t="s">
+      <c r="F70" s="123" t="s">
         <v>855</v>
       </c>
       <c r="G70" s="59"/>
@@ -27368,8 +27368,8 @@
       <c r="D71" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E71" s="125"/>
-      <c r="F71" s="125"/>
+      <c r="E71" s="123"/>
+      <c r="F71" s="123"/>
       <c r="G71" s="59"/>
     </row>
     <row r="72" spans="1:7" ht="78" x14ac:dyDescent="0.3">
@@ -27677,10 +27677,10 @@
         <v>8</v>
       </c>
       <c r="E87" s="29" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="F87" s="113" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="G87" s="59"/>
     </row>
@@ -28038,7 +28038,7 @@
         <v>6</v>
       </c>
       <c r="E106" s="113" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="F106" s="27" t="s">
         <v>29</v>
@@ -28187,10 +28187,10 @@
       <c r="D114" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="E114" s="129" t="s">
+      <c r="E114" s="128" t="s">
         <v>468</v>
       </c>
-      <c r="F114" s="118" t="s">
+      <c r="F114" s="120" t="s">
         <v>469</v>
       </c>
     </row>
@@ -28207,8 +28207,8 @@
       <c r="D115" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="E115" s="129"/>
-      <c r="F115" s="118"/>
+      <c r="E115" s="128"/>
+      <c r="F115" s="120"/>
     </row>
     <row r="116" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A116" s="22" t="s">
@@ -28344,10 +28344,10 @@
         <v>8</v>
       </c>
       <c r="E122" s="114" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="F122" s="114" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="123" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
@@ -28413,10 +28413,10 @@
       <c r="D126" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="E126" s="118" t="s">
+      <c r="E126" s="120" t="s">
         <v>470</v>
       </c>
-      <c r="F126" s="119" t="s">
+      <c r="F126" s="121" t="s">
         <v>471</v>
       </c>
     </row>
@@ -28433,8 +28433,8 @@
       <c r="D127" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="E127" s="118"/>
-      <c r="F127" s="120"/>
+      <c r="E127" s="120"/>
+      <c r="F127" s="122"/>
     </row>
     <row r="128" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A128" s="22" t="s">
@@ -28518,10 +28518,10 @@
       <c r="D132" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="E132" s="118" t="s">
+      <c r="E132" s="120" t="s">
         <v>472</v>
       </c>
-      <c r="F132" s="118" t="s">
+      <c r="F132" s="120" t="s">
         <v>473</v>
       </c>
     </row>
@@ -28538,8 +28538,8 @@
       <c r="D133" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="E133" s="118"/>
-      <c r="F133" s="118"/>
+      <c r="E133" s="120"/>
+      <c r="F133" s="120"/>
     </row>
     <row r="134" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A134" s="22" t="s">
@@ -28554,8 +28554,8 @@
       <c r="D134" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="E134" s="118"/>
-      <c r="F134" s="118"/>
+      <c r="E134" s="120"/>
+      <c r="F134" s="120"/>
     </row>
     <row r="135" spans="1:6" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A135" s="22" t="s">
@@ -28723,7 +28723,7 @@
       <c r="E143" s="27" t="s">
         <v>474</v>
       </c>
-      <c r="F143" s="125" t="s">
+      <c r="F143" s="123" t="s">
         <v>357</v>
       </c>
     </row>
@@ -28743,7 +28743,7 @@
       <c r="E144" s="27" t="s">
         <v>475</v>
       </c>
-      <c r="F144" s="125"/>
+      <c r="F144" s="123"/>
     </row>
     <row r="145" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A145" s="22" t="s">
@@ -28858,10 +28858,10 @@
       <c r="D150" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="E150" s="119" t="s">
+      <c r="E150" s="121" t="s">
         <v>481</v>
       </c>
-      <c r="F150" s="119" t="s">
+      <c r="F150" s="121" t="s">
         <v>482</v>
       </c>
       <c r="G150" s="63"/>
@@ -28879,8 +28879,8 @@
       <c r="D151" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="E151" s="120"/>
-      <c r="F151" s="120"/>
+      <c r="E151" s="122"/>
+      <c r="F151" s="122"/>
       <c r="G151" s="59"/>
     </row>
     <row r="152" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
@@ -28896,10 +28896,10 @@
       <c r="D152" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="E152" s="128" t="s">
+      <c r="E152" s="129" t="s">
         <v>483</v>
       </c>
-      <c r="F152" s="128" t="s">
+      <c r="F152" s="129" t="s">
         <v>463</v>
       </c>
     </row>
@@ -28916,8 +28916,8 @@
       <c r="D153" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="E153" s="128"/>
-      <c r="F153" s="128"/>
+      <c r="E153" s="129"/>
+      <c r="F153" s="129"/>
     </row>
     <row r="154" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A154" s="22" t="s">
@@ -29083,7 +29083,7 @@
         <v>8</v>
       </c>
       <c r="E162" s="29" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="F162" s="29" t="s">
         <v>170</v>
@@ -29191,12 +29191,22 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="E152:E153"/>
+    <mergeCell ref="F152:F153"/>
+    <mergeCell ref="A155:F155"/>
+    <mergeCell ref="A131:F131"/>
+    <mergeCell ref="E132:E134"/>
+    <mergeCell ref="F132:F134"/>
+    <mergeCell ref="A142:F142"/>
+    <mergeCell ref="F143:F144"/>
+    <mergeCell ref="E150:E151"/>
+    <mergeCell ref="F150:F151"/>
+    <mergeCell ref="A113:F113"/>
+    <mergeCell ref="E114:E115"/>
+    <mergeCell ref="F114:F115"/>
+    <mergeCell ref="A125:F125"/>
+    <mergeCell ref="E126:E127"/>
+    <mergeCell ref="F126:F127"/>
     <mergeCell ref="A102:F102"/>
     <mergeCell ref="A19:F19"/>
     <mergeCell ref="A33:F33"/>
@@ -29210,22 +29220,12 @@
     <mergeCell ref="F70:F71"/>
     <mergeCell ref="A82:F82"/>
     <mergeCell ref="A91:F91"/>
-    <mergeCell ref="A113:F113"/>
-    <mergeCell ref="E114:E115"/>
-    <mergeCell ref="F114:F115"/>
-    <mergeCell ref="A125:F125"/>
-    <mergeCell ref="E126:E127"/>
-    <mergeCell ref="F126:F127"/>
-    <mergeCell ref="E152:E153"/>
-    <mergeCell ref="F152:F153"/>
-    <mergeCell ref="A155:F155"/>
-    <mergeCell ref="A131:F131"/>
-    <mergeCell ref="E132:E134"/>
-    <mergeCell ref="F132:F134"/>
-    <mergeCell ref="A142:F142"/>
-    <mergeCell ref="F143:F144"/>
-    <mergeCell ref="E150:E151"/>
-    <mergeCell ref="F150:F151"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="F11:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -29289,10 +29289,10 @@
       <c r="D3" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="125" t="s">
+      <c r="E3" s="123" t="s">
         <v>968</v>
       </c>
-      <c r="F3" s="123" t="s">
+      <c r="F3" s="125" t="s">
         <v>484</v>
       </c>
     </row>
@@ -29309,8 +29309,8 @@
       <c r="D4" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="125"/>
-      <c r="F4" s="124"/>
+      <c r="E4" s="123"/>
+      <c r="F4" s="126"/>
     </row>
     <row r="5" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
@@ -29406,7 +29406,7 @@
         <v>8</v>
       </c>
       <c r="E9" s="43" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="F9" s="31" t="s">
         <v>486</v>
@@ -29435,10 +29435,10 @@
       <c r="D11" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="123" t="s">
+      <c r="E11" s="125" t="s">
         <v>487</v>
       </c>
-      <c r="F11" s="123" t="s">
+      <c r="F11" s="125" t="s">
         <v>488</v>
       </c>
     </row>
@@ -29455,8 +29455,8 @@
       <c r="D12" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="126"/>
-      <c r="F12" s="126"/>
+      <c r="E12" s="127"/>
+      <c r="F12" s="127"/>
     </row>
     <row r="13" spans="1:6" ht="110.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="22" t="s">
@@ -29471,8 +29471,8 @@
       <c r="D13" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="124"/>
-      <c r="F13" s="124"/>
+      <c r="E13" s="126"/>
+      <c r="F13" s="126"/>
     </row>
     <row r="14" spans="1:6" ht="113.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="22" t="s">
@@ -29986,10 +29986,10 @@
         <v>8</v>
       </c>
       <c r="E40" s="43" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="F40" s="31" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
@@ -30398,7 +30398,7 @@
         <v>8</v>
       </c>
       <c r="E62" s="39" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="F62" s="39" t="s">
         <v>170</v>
@@ -30537,10 +30537,10 @@
       <c r="D70" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E70" s="123" t="s">
+      <c r="E70" s="125" t="s">
         <v>497</v>
       </c>
-      <c r="F70" s="119" t="s">
+      <c r="F70" s="121" t="s">
         <v>498</v>
       </c>
     </row>
@@ -30557,7 +30557,7 @@
       <c r="D71" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E71" s="124"/>
+      <c r="E71" s="126"/>
       <c r="F71" s="130"/>
     </row>
     <row r="72" spans="1:6" ht="126" customHeight="1" x14ac:dyDescent="0.3">
@@ -30864,10 +30864,10 @@
         <v>8</v>
       </c>
       <c r="E87" s="91" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="F87" s="113" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="102.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -31220,7 +31220,7 @@
         <v>6</v>
       </c>
       <c r="E106" s="113" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="F106" s="113" t="s">
         <v>29</v>
@@ -31530,10 +31530,10 @@
         <v>8</v>
       </c>
       <c r="E122" s="114" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="F122" s="114" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="123" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
@@ -31599,10 +31599,10 @@
       <c r="D126" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="E126" s="118" t="s">
+      <c r="E126" s="120" t="s">
         <v>504</v>
       </c>
-      <c r="F126" s="119" t="s">
+      <c r="F126" s="121" t="s">
         <v>505</v>
       </c>
     </row>
@@ -31619,8 +31619,8 @@
       <c r="D127" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="E127" s="118"/>
-      <c r="F127" s="120"/>
+      <c r="E127" s="120"/>
+      <c r="F127" s="122"/>
     </row>
     <row r="128" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A128" s="22" t="s">
@@ -31703,10 +31703,10 @@
       <c r="D132" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="E132" s="118" t="s">
+      <c r="E132" s="120" t="s">
         <v>506</v>
       </c>
-      <c r="F132" s="119" t="s">
+      <c r="F132" s="121" t="s">
         <v>507</v>
       </c>
     </row>
@@ -31723,8 +31723,8 @@
       <c r="D133" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="E133" s="118"/>
-      <c r="F133" s="120"/>
+      <c r="E133" s="120"/>
+      <c r="F133" s="122"/>
     </row>
     <row r="134" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A134" s="22" t="s">
@@ -32030,10 +32030,10 @@
         <v>8</v>
       </c>
       <c r="E149" s="43" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F149" s="113" t="s">
         <v>1071</v>
-      </c>
-      <c r="F149" s="113" t="s">
-        <v>1072</v>
       </c>
     </row>
     <row r="150" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
@@ -32130,7 +32130,7 @@
         <v>8</v>
       </c>
       <c r="E154" s="95" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="F154" s="95" t="s">
         <v>886</v>
@@ -32219,10 +32219,10 @@
       <c r="D159" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="E159" s="118" t="s">
+      <c r="E159" s="120" t="s">
         <v>514</v>
       </c>
-      <c r="F159" s="119" t="s">
+      <c r="F159" s="121" t="s">
         <v>886</v>
       </c>
     </row>
@@ -32239,8 +32239,8 @@
       <c r="D160" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="E160" s="118"/>
-      <c r="F160" s="120"/>
+      <c r="E160" s="120"/>
+      <c r="F160" s="122"/>
     </row>
     <row r="161" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A161" s="22" t="s">
@@ -32276,7 +32276,7 @@
         <v>8</v>
       </c>
       <c r="E162" s="39" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="F162" s="39" t="s">
         <v>170</v>
@@ -32356,10 +32356,10 @@
         <v>8</v>
       </c>
       <c r="E166" s="113" t="s">
+        <v>1072</v>
+      </c>
+      <c r="F166" s="113" t="s">
         <v>1073</v>
-      </c>
-      <c r="F166" s="113" t="s">
-        <v>1074</v>
       </c>
     </row>
     <row r="167" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
@@ -32384,16 +32384,12 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A142:F142"/>
-    <mergeCell ref="A155:F155"/>
-    <mergeCell ref="E159:E160"/>
-    <mergeCell ref="F159:F160"/>
-    <mergeCell ref="A125:F125"/>
-    <mergeCell ref="E126:E127"/>
-    <mergeCell ref="F126:F127"/>
-    <mergeCell ref="A131:F131"/>
-    <mergeCell ref="E132:E133"/>
-    <mergeCell ref="F132:F133"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="F11:F13"/>
     <mergeCell ref="A113:F113"/>
     <mergeCell ref="A19:F19"/>
     <mergeCell ref="A33:F33"/>
@@ -32406,12 +32402,16 @@
     <mergeCell ref="A82:F82"/>
     <mergeCell ref="A91:F91"/>
     <mergeCell ref="A102:F102"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="A142:F142"/>
+    <mergeCell ref="A155:F155"/>
+    <mergeCell ref="E159:E160"/>
+    <mergeCell ref="F159:F160"/>
+    <mergeCell ref="A125:F125"/>
+    <mergeCell ref="E126:E127"/>
+    <mergeCell ref="F126:F127"/>
+    <mergeCell ref="A131:F131"/>
+    <mergeCell ref="E132:E133"/>
+    <mergeCell ref="F132:F133"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -32556,10 +32556,10 @@
         <v>8</v>
       </c>
       <c r="E7" s="88" t="s">
+        <v>1031</v>
+      </c>
+      <c r="F7" s="88" t="s">
         <v>1032</v>
-      </c>
-      <c r="F7" s="88" t="s">
-        <v>1033</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="93.6" x14ac:dyDescent="0.3">
@@ -32596,10 +32596,10 @@
         <v>8</v>
       </c>
       <c r="E9" s="87" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="F9" s="87" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -32625,10 +32625,10 @@
       <c r="D11" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="125" t="s">
+      <c r="E11" s="123" t="s">
         <v>972</v>
       </c>
-      <c r="F11" s="125" t="s">
+      <c r="F11" s="123" t="s">
         <v>914</v>
       </c>
     </row>
@@ -32645,8 +32645,8 @@
       <c r="D12" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="125"/>
-      <c r="F12" s="125"/>
+      <c r="E12" s="123"/>
+      <c r="F12" s="123"/>
     </row>
     <row r="13" spans="1:6" ht="150.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="22" t="s">
@@ -32682,10 +32682,10 @@
         <v>6</v>
       </c>
       <c r="E14" s="87" t="s">
+        <v>1038</v>
+      </c>
+      <c r="F14" s="87" t="s">
         <v>1039</v>
-      </c>
-      <c r="F14" s="87" t="s">
-        <v>1040</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="109.2" x14ac:dyDescent="0.3">
@@ -32791,10 +32791,10 @@
       <c r="D20" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E20" s="118" t="s">
+      <c r="E20" s="120" t="s">
         <v>757</v>
       </c>
-      <c r="F20" s="118" t="s">
+      <c r="F20" s="120" t="s">
         <v>758</v>
       </c>
     </row>
@@ -32811,8 +32811,8 @@
       <c r="D21" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="118"/>
-      <c r="F21" s="118"/>
+      <c r="E21" s="120"/>
+      <c r="F21" s="120"/>
     </row>
     <row r="22" spans="1:6" ht="200.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="22" t="s">
@@ -33475,10 +33475,10 @@
       <c r="D56" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E56" s="125" t="s">
+      <c r="E56" s="123" t="s">
         <v>764</v>
       </c>
-      <c r="F56" s="125" t="s">
+      <c r="F56" s="123" t="s">
         <v>765</v>
       </c>
     </row>
@@ -33495,8 +33495,8 @@
       <c r="D57" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E57" s="125"/>
-      <c r="F57" s="125"/>
+      <c r="E57" s="123"/>
+      <c r="F57" s="123"/>
     </row>
     <row r="58" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A58" s="22" t="s">
@@ -33592,7 +33592,7 @@
         <v>8</v>
       </c>
       <c r="E62" s="87" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="F62" s="87" t="s">
         <v>170</v>
@@ -33731,10 +33731,10 @@
       <c r="D70" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E70" s="125" t="s">
+      <c r="E70" s="123" t="s">
         <v>819</v>
       </c>
-      <c r="F70" s="125" t="s">
+      <c r="F70" s="123" t="s">
         <v>892</v>
       </c>
     </row>
@@ -33751,8 +33751,8 @@
       <c r="D71" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E71" s="125"/>
-      <c r="F71" s="125"/>
+      <c r="E71" s="123"/>
+      <c r="F71" s="123"/>
     </row>
     <row r="72" spans="1:6" ht="78" x14ac:dyDescent="0.3">
       <c r="A72" s="22" t="s">
@@ -33807,10 +33807,10 @@
       <c r="D74" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E74" s="118" t="s">
+      <c r="E74" s="120" t="s">
         <v>874</v>
       </c>
-      <c r="F74" s="118" t="s">
+      <c r="F74" s="120" t="s">
         <v>767</v>
       </c>
     </row>
@@ -33827,8 +33827,8 @@
       <c r="D75" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E75" s="118"/>
-      <c r="F75" s="118"/>
+      <c r="E75" s="120"/>
+      <c r="F75" s="120"/>
     </row>
     <row r="76" spans="1:6" ht="78" x14ac:dyDescent="0.3">
       <c r="A76" s="22" t="s">
@@ -34054,10 +34054,10 @@
         <v>8</v>
       </c>
       <c r="E87" s="88" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="F87" s="88" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="78" x14ac:dyDescent="0.3">
@@ -34163,10 +34163,10 @@
       <c r="D93" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E93" s="119" t="s">
+      <c r="E93" s="121" t="s">
         <v>987</v>
       </c>
-      <c r="F93" s="119" t="s">
+      <c r="F93" s="121" t="s">
         <v>769</v>
       </c>
     </row>
@@ -34183,8 +34183,8 @@
       <c r="D94" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E94" s="120"/>
-      <c r="F94" s="120"/>
+      <c r="E94" s="122"/>
+      <c r="F94" s="122"/>
     </row>
     <row r="95" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A95" s="22" t="s">
@@ -34559,10 +34559,10 @@
       <c r="D114" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E114" s="118" t="s">
+      <c r="E114" s="120" t="s">
         <v>777</v>
       </c>
-      <c r="F114" s="118" t="s">
+      <c r="F114" s="120" t="s">
         <v>778</v>
       </c>
     </row>
@@ -34579,8 +34579,8 @@
       <c r="D115" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E115" s="118"/>
-      <c r="F115" s="118"/>
+      <c r="E115" s="120"/>
+      <c r="F115" s="120"/>
     </row>
     <row r="116" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A116" s="22" t="s">
@@ -34716,10 +34716,10 @@
         <v>8</v>
       </c>
       <c r="E122" s="114" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="F122" s="114" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="123" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
@@ -35124,7 +35124,7 @@
       <c r="E144" s="88" t="s">
         <v>790</v>
       </c>
-      <c r="F144" s="125" t="s">
+      <c r="F144" s="123" t="s">
         <v>35</v>
       </c>
     </row>
@@ -35144,7 +35144,7 @@
       <c r="E145" s="88" t="s">
         <v>791</v>
       </c>
-      <c r="F145" s="125"/>
+      <c r="F145" s="123"/>
     </row>
     <row r="146" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A146" s="22" t="s">
@@ -35316,7 +35316,7 @@
         <v>8</v>
       </c>
       <c r="E154" s="95" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F154" s="95" t="s">
         <v>887</v>
@@ -35346,10 +35346,10 @@
         <v>8</v>
       </c>
       <c r="E156" s="88" t="s">
+        <v>1097</v>
+      </c>
+      <c r="F156" s="88" t="s">
         <v>1098</v>
-      </c>
-      <c r="F156" s="88" t="s">
-        <v>1099</v>
       </c>
     </row>
     <row r="157" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
@@ -35466,7 +35466,7 @@
         <v>8</v>
       </c>
       <c r="E162" s="87" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="F162" s="87" t="s">
         <v>560</v>
@@ -35544,10 +35544,10 @@
         <v>8</v>
       </c>
       <c r="E166" s="113" t="s">
+        <v>1099</v>
+      </c>
+      <c r="F166" s="113" t="s">
         <v>1100</v>
-      </c>
-      <c r="F166" s="113" t="s">
-        <v>1101</v>
       </c>
     </row>
     <row r="167" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
@@ -35572,6 +35572,28 @@
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="E152:E153"/>
+    <mergeCell ref="F152:F153"/>
+    <mergeCell ref="A155:F155"/>
+    <mergeCell ref="A125:F125"/>
+    <mergeCell ref="E126:E127"/>
+    <mergeCell ref="F126:F127"/>
+    <mergeCell ref="A131:F131"/>
+    <mergeCell ref="A142:F142"/>
+    <mergeCell ref="F144:F145"/>
+    <mergeCell ref="E114:E115"/>
+    <mergeCell ref="F114:F115"/>
+    <mergeCell ref="A69:F69"/>
+    <mergeCell ref="E70:E71"/>
+    <mergeCell ref="F70:F71"/>
+    <mergeCell ref="E74:E75"/>
+    <mergeCell ref="F74:F75"/>
+    <mergeCell ref="A82:F82"/>
+    <mergeCell ref="A91:F91"/>
+    <mergeCell ref="E93:E94"/>
+    <mergeCell ref="F93:F94"/>
+    <mergeCell ref="A102:F102"/>
+    <mergeCell ref="A113:F113"/>
     <mergeCell ref="A63:F63"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A10:F10"/>
@@ -35585,28 +35607,6 @@
     <mergeCell ref="A54:F54"/>
     <mergeCell ref="E56:E57"/>
     <mergeCell ref="F56:F57"/>
-    <mergeCell ref="E114:E115"/>
-    <mergeCell ref="F114:F115"/>
-    <mergeCell ref="A69:F69"/>
-    <mergeCell ref="E70:E71"/>
-    <mergeCell ref="F70:F71"/>
-    <mergeCell ref="E74:E75"/>
-    <mergeCell ref="F74:F75"/>
-    <mergeCell ref="A82:F82"/>
-    <mergeCell ref="A91:F91"/>
-    <mergeCell ref="E93:E94"/>
-    <mergeCell ref="F93:F94"/>
-    <mergeCell ref="A102:F102"/>
-    <mergeCell ref="A113:F113"/>
-    <mergeCell ref="E152:E153"/>
-    <mergeCell ref="F152:F153"/>
-    <mergeCell ref="A155:F155"/>
-    <mergeCell ref="A125:F125"/>
-    <mergeCell ref="E126:E127"/>
-    <mergeCell ref="F126:F127"/>
-    <mergeCell ref="A131:F131"/>
-    <mergeCell ref="A142:F142"/>
-    <mergeCell ref="F144:F145"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -35821,10 +35821,10 @@
       <c r="D11" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="123" t="s">
+      <c r="E11" s="125" t="s">
         <v>711</v>
       </c>
-      <c r="F11" s="125" t="s">
+      <c r="F11" s="123" t="s">
         <v>712</v>
       </c>
     </row>
@@ -35841,8 +35841,8 @@
       <c r="D12" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="124"/>
-      <c r="F12" s="125"/>
+      <c r="E12" s="126"/>
+      <c r="F12" s="123"/>
     </row>
     <row r="13" spans="1:6" ht="117" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="22" t="s">
@@ -35987,10 +35987,10 @@
       <c r="D20" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="118" t="s">
+      <c r="E20" s="120" t="s">
         <v>810</v>
       </c>
-      <c r="F20" s="118" t="s">
+      <c r="F20" s="120" t="s">
         <v>842</v>
       </c>
     </row>
@@ -36007,8 +36007,8 @@
       <c r="D21" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="118"/>
-      <c r="F21" s="118"/>
+      <c r="E21" s="120"/>
+      <c r="F21" s="120"/>
     </row>
     <row r="22" spans="1:6" ht="118.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="22" t="s">
@@ -36671,10 +36671,10 @@
       <c r="D56" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E56" s="123" t="s">
+      <c r="E56" s="125" t="s">
         <v>808</v>
       </c>
-      <c r="F56" s="123" t="s">
+      <c r="F56" s="125" t="s">
         <v>809</v>
       </c>
     </row>
@@ -36691,8 +36691,8 @@
       <c r="D57" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E57" s="124"/>
-      <c r="F57" s="124"/>
+      <c r="E57" s="126"/>
+      <c r="F57" s="126"/>
     </row>
     <row r="58" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A58" s="22" t="s">
@@ -36788,7 +36788,7 @@
         <v>8</v>
       </c>
       <c r="E62" s="79" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="F62" s="79" t="s">
         <v>380</v>
@@ -36927,10 +36927,10 @@
       <c r="D70" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E70" s="123" t="s">
+      <c r="E70" s="125" t="s">
         <v>723</v>
       </c>
-      <c r="F70" s="123" t="s">
+      <c r="F70" s="125" t="s">
         <v>724</v>
       </c>
     </row>
@@ -36947,8 +36947,8 @@
       <c r="D71" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E71" s="124"/>
-      <c r="F71" s="124"/>
+      <c r="E71" s="126"/>
+      <c r="F71" s="126"/>
     </row>
     <row r="72" spans="1:6" ht="78" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="22" t="s">
@@ -37003,10 +37003,10 @@
       <c r="D74" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E74" s="119" t="s">
+      <c r="E74" s="121" t="s">
         <v>726</v>
       </c>
-      <c r="F74" s="119" t="s">
+      <c r="F74" s="121" t="s">
         <v>725</v>
       </c>
     </row>
@@ -37023,8 +37023,8 @@
       <c r="D75" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E75" s="120"/>
-      <c r="F75" s="120"/>
+      <c r="E75" s="122"/>
+      <c r="F75" s="122"/>
     </row>
     <row r="76" spans="1:6" ht="78" x14ac:dyDescent="0.3">
       <c r="A76" s="22" t="s">
@@ -37250,10 +37250,10 @@
         <v>8</v>
       </c>
       <c r="E87" s="81" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="F87" s="81" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="78" customHeight="1" x14ac:dyDescent="0.3">
@@ -37759,10 +37759,10 @@
       <c r="D114" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E114" s="118" t="s">
+      <c r="E114" s="120" t="s">
         <v>734</v>
       </c>
-      <c r="F114" s="119" t="s">
+      <c r="F114" s="121" t="s">
         <v>735</v>
       </c>
     </row>
@@ -37779,8 +37779,8 @@
       <c r="D115" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E115" s="118"/>
-      <c r="F115" s="120"/>
+      <c r="E115" s="120"/>
+      <c r="F115" s="122"/>
     </row>
     <row r="116" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A116" s="22" t="s">
@@ -37916,10 +37916,10 @@
         <v>8</v>
       </c>
       <c r="E122" s="114" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="F122" s="114" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="123" spans="1:6" ht="142.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -38666,7 +38666,7 @@
         <v>8</v>
       </c>
       <c r="E162" s="79" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="F162" s="79" t="s">
         <v>751</v>
@@ -38774,28 +38774,6 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="E70:E71"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A44:F44"/>
-    <mergeCell ref="A54:F54"/>
-    <mergeCell ref="A63:F63"/>
-    <mergeCell ref="A69:F69"/>
-    <mergeCell ref="F70:F71"/>
-    <mergeCell ref="E56:E57"/>
-    <mergeCell ref="F56:F57"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="F74:F75"/>
-    <mergeCell ref="A82:F82"/>
-    <mergeCell ref="A91:F91"/>
-    <mergeCell ref="A102:F102"/>
-    <mergeCell ref="A113:F113"/>
-    <mergeCell ref="E74:E75"/>
     <mergeCell ref="F152:F153"/>
     <mergeCell ref="A155:F155"/>
     <mergeCell ref="F114:F115"/>
@@ -38806,6 +38784,28 @@
     <mergeCell ref="E114:E115"/>
     <mergeCell ref="E126:E127"/>
     <mergeCell ref="E152:E153"/>
+    <mergeCell ref="F74:F75"/>
+    <mergeCell ref="A82:F82"/>
+    <mergeCell ref="A91:F91"/>
+    <mergeCell ref="A102:F102"/>
+    <mergeCell ref="A113:F113"/>
+    <mergeCell ref="E74:E75"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="E70:E71"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A44:F44"/>
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="A63:F63"/>
+    <mergeCell ref="A69:F69"/>
+    <mergeCell ref="F70:F71"/>
+    <mergeCell ref="E56:E57"/>
+    <mergeCell ref="F56:F57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -38816,7 +38816,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:F167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A151" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E154" sqref="E154"/>
     </sheetView>
   </sheetViews>
@@ -38869,10 +38869,10 @@
       <c r="D3" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="125" t="s">
+      <c r="E3" s="123" t="s">
         <v>970</v>
       </c>
-      <c r="F3" s="123" t="s">
+      <c r="F3" s="125" t="s">
         <v>971</v>
       </c>
     </row>
@@ -38889,8 +38889,8 @@
       <c r="D4" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="125"/>
-      <c r="F4" s="124"/>
+      <c r="E4" s="123"/>
+      <c r="F4" s="126"/>
     </row>
     <row r="5" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
@@ -39015,10 +39015,10 @@
       <c r="D11" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="123" t="s">
+      <c r="E11" s="125" t="s">
         <v>926</v>
       </c>
-      <c r="F11" s="123" t="s">
+      <c r="F11" s="125" t="s">
         <v>663</v>
       </c>
     </row>
@@ -39035,8 +39035,8 @@
       <c r="D12" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="126"/>
-      <c r="F12" s="126"/>
+      <c r="E12" s="127"/>
+      <c r="F12" s="127"/>
     </row>
     <row r="13" spans="1:6" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A13" s="22" t="s">
@@ -39051,8 +39051,8 @@
       <c r="D13" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="124"/>
-      <c r="F13" s="124"/>
+      <c r="E13" s="126"/>
+      <c r="F13" s="126"/>
     </row>
     <row r="14" spans="1:6" ht="115.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="22" t="s">
@@ -39177,10 +39177,10 @@
       <c r="D20" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="E20" s="125" t="s">
+      <c r="E20" s="123" t="s">
         <v>974</v>
       </c>
-      <c r="F20" s="123" t="s">
+      <c r="F20" s="125" t="s">
         <v>975</v>
       </c>
     </row>
@@ -39197,8 +39197,8 @@
       <c r="D21" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="125"/>
-      <c r="F21" s="124"/>
+      <c r="E21" s="123"/>
+      <c r="F21" s="126"/>
     </row>
     <row r="22" spans="1:6" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="22" t="s">
@@ -40011,10 +40011,10 @@
       <c r="D64" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="E64" s="123" t="s">
+      <c r="E64" s="125" t="s">
         <v>674</v>
       </c>
-      <c r="F64" s="123" t="s">
+      <c r="F64" s="125" t="s">
         <v>675</v>
       </c>
     </row>
@@ -40031,8 +40031,8 @@
       <c r="D65" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="E65" s="124"/>
-      <c r="F65" s="124"/>
+      <c r="E65" s="126"/>
+      <c r="F65" s="126"/>
     </row>
     <row r="66" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A66" s="22" t="s">
@@ -40117,10 +40117,10 @@
       <c r="D70" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="E70" s="125" t="s">
+      <c r="E70" s="123" t="s">
         <v>980</v>
       </c>
-      <c r="F70" s="123" t="s">
+      <c r="F70" s="125" t="s">
         <v>981</v>
       </c>
     </row>
@@ -40137,8 +40137,8 @@
       <c r="D71" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="E71" s="125"/>
-      <c r="F71" s="124"/>
+      <c r="E71" s="123"/>
+      <c r="F71" s="126"/>
     </row>
     <row r="72" spans="1:6" ht="78" x14ac:dyDescent="0.3">
       <c r="A72" s="22" t="s">
@@ -40193,10 +40193,10 @@
       <c r="D74" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="E74" s="123" t="s">
+      <c r="E74" s="125" t="s">
         <v>676</v>
       </c>
-      <c r="F74" s="126" t="s">
+      <c r="F74" s="127" t="s">
         <v>195</v>
       </c>
     </row>
@@ -40213,8 +40213,8 @@
       <c r="D75" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="E75" s="124"/>
-      <c r="F75" s="124"/>
+      <c r="E75" s="126"/>
+      <c r="F75" s="126"/>
     </row>
     <row r="76" spans="1:6" ht="78" x14ac:dyDescent="0.3">
       <c r="A76" s="22" t="s">
@@ -40440,10 +40440,10 @@
         <v>8</v>
       </c>
       <c r="E87" s="84" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="F87" s="84" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="78" x14ac:dyDescent="0.3">
@@ -40800,7 +40800,7 @@
         <v>6</v>
       </c>
       <c r="E106" s="113" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="F106" s="113" t="s">
         <v>29</v>
@@ -40949,10 +40949,10 @@
       <c r="D114" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="E114" s="123" t="s">
+      <c r="E114" s="125" t="s">
         <v>684</v>
       </c>
-      <c r="F114" s="123" t="s">
+      <c r="F114" s="125" t="s">
         <v>685</v>
       </c>
     </row>
@@ -40969,8 +40969,8 @@
       <c r="D115" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="E115" s="124"/>
-      <c r="F115" s="124"/>
+      <c r="E115" s="126"/>
+      <c r="F115" s="126"/>
     </row>
     <row r="116" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A116" s="22" t="s">
@@ -41106,10 +41106,10 @@
         <v>8</v>
       </c>
       <c r="E122" s="114" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="F122" s="114" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="123" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
@@ -41966,6 +41966,22 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="E114:E115"/>
+    <mergeCell ref="E126:E127"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A44:F44"/>
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="F74:F75"/>
+    <mergeCell ref="A82:F82"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="F20:F21"/>
     <mergeCell ref="A155:F155"/>
     <mergeCell ref="E64:E65"/>
     <mergeCell ref="E70:E71"/>
@@ -41982,22 +41998,6 @@
     <mergeCell ref="F126:F127"/>
     <mergeCell ref="A131:F131"/>
     <mergeCell ref="A142:F142"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="F11:F13"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="E114:E115"/>
-    <mergeCell ref="E126:E127"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A44:F44"/>
-    <mergeCell ref="A54:F54"/>
-    <mergeCell ref="F74:F75"/>
-    <mergeCell ref="A82:F82"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -42062,10 +42062,10 @@
       <c r="D3" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="123" t="s">
+      <c r="E3" s="125" t="s">
         <v>516</v>
       </c>
-      <c r="F3" s="123" t="s">
+      <c r="F3" s="125" t="s">
         <v>517</v>
       </c>
     </row>
@@ -42082,8 +42082,8 @@
       <c r="D4" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="124"/>
-      <c r="F4" s="124"/>
+      <c r="E4" s="126"/>
+      <c r="F4" s="126"/>
     </row>
     <row r="5" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
@@ -42208,10 +42208,10 @@
       <c r="D11" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="123" t="s">
+      <c r="E11" s="125" t="s">
         <v>838</v>
       </c>
-      <c r="F11" s="123" t="s">
+      <c r="F11" s="125" t="s">
         <v>525</v>
       </c>
     </row>
@@ -42228,8 +42228,8 @@
       <c r="D12" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="126"/>
-      <c r="F12" s="126"/>
+      <c r="E12" s="127"/>
+      <c r="F12" s="127"/>
     </row>
     <row r="13" spans="1:6" ht="105.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="22" t="s">
@@ -42244,8 +42244,8 @@
       <c r="D13" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="126"/>
-      <c r="F13" s="126"/>
+      <c r="E13" s="127"/>
+      <c r="F13" s="127"/>
     </row>
     <row r="14" spans="1:6" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A14" s="22" t="s">
@@ -42260,8 +42260,8 @@
       <c r="D14" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="124"/>
-      <c r="F14" s="124"/>
+      <c r="E14" s="126"/>
+      <c r="F14" s="126"/>
     </row>
     <row r="15" spans="1:6" ht="109.2" x14ac:dyDescent="0.3">
       <c r="A15" s="22" t="s">
@@ -42366,10 +42366,10 @@
       <c r="D20" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="E20" s="123" t="s">
+      <c r="E20" s="125" t="s">
         <v>843</v>
       </c>
-      <c r="F20" s="123" t="s">
+      <c r="F20" s="125" t="s">
         <v>526</v>
       </c>
     </row>
@@ -42386,8 +42386,8 @@
       <c r="D21" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="124"/>
-      <c r="F21" s="124"/>
+      <c r="E21" s="126"/>
+      <c r="F21" s="126"/>
     </row>
     <row r="22" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A22" s="22" t="s">
@@ -43310,10 +43310,10 @@
       <c r="D70" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="E70" s="123" t="s">
+      <c r="E70" s="125" t="s">
         <v>533</v>
       </c>
-      <c r="F70" s="123" t="s">
+      <c r="F70" s="125" t="s">
         <v>534</v>
       </c>
     </row>
@@ -43330,8 +43330,8 @@
       <c r="D71" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="E71" s="124"/>
-      <c r="F71" s="124"/>
+      <c r="E71" s="126"/>
+      <c r="F71" s="126"/>
     </row>
     <row r="72" spans="1:6" ht="78" x14ac:dyDescent="0.3">
       <c r="A72" s="22" t="s">
@@ -43386,10 +43386,10 @@
       <c r="D74" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="E74" s="118" t="s">
+      <c r="E74" s="120" t="s">
         <v>535</v>
       </c>
-      <c r="F74" s="118" t="s">
+      <c r="F74" s="120" t="s">
         <v>535</v>
       </c>
     </row>
@@ -43406,8 +43406,8 @@
       <c r="D75" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="E75" s="118"/>
-      <c r="F75" s="118"/>
+      <c r="E75" s="120"/>
+      <c r="F75" s="120"/>
     </row>
     <row r="76" spans="1:6" ht="78" x14ac:dyDescent="0.3">
       <c r="A76" s="22" t="s">
@@ -43633,10 +43633,10 @@
         <v>8</v>
       </c>
       <c r="E87" s="39" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="F87" s="31" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="78" x14ac:dyDescent="0.3">
@@ -43742,10 +43742,10 @@
       <c r="D93" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E93" s="123" t="s">
+      <c r="E93" s="125" t="s">
         <v>988</v>
       </c>
-      <c r="F93" s="123" t="s">
+      <c r="F93" s="125" t="s">
         <v>531</v>
       </c>
     </row>
@@ -43762,8 +43762,8 @@
       <c r="D94" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="E94" s="124"/>
-      <c r="F94" s="124"/>
+      <c r="E94" s="126"/>
+      <c r="F94" s="126"/>
     </row>
     <row r="95" spans="1:6" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="22" t="s">
@@ -44138,10 +44138,10 @@
       <c r="D114" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="E114" s="125" t="s">
+      <c r="E114" s="123" t="s">
         <v>547</v>
       </c>
-      <c r="F114" s="123" t="s">
+      <c r="F114" s="125" t="s">
         <v>548</v>
       </c>
     </row>
@@ -44158,8 +44158,8 @@
       <c r="D115" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="E115" s="125"/>
-      <c r="F115" s="124"/>
+      <c r="E115" s="123"/>
+      <c r="F115" s="126"/>
     </row>
     <row r="116" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A116" s="22" t="s">
@@ -44295,10 +44295,10 @@
         <v>8</v>
       </c>
       <c r="E122" s="39" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="F122" s="39" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="123" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
@@ -45047,7 +45047,7 @@
         <v>8</v>
       </c>
       <c r="E162" s="39" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="F162" s="39" t="s">
         <v>560</v>
@@ -45155,14 +45155,18 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="A142:F142"/>
-    <mergeCell ref="A155:F155"/>
-    <mergeCell ref="E114:E115"/>
-    <mergeCell ref="F114:F115"/>
-    <mergeCell ref="A125:F125"/>
-    <mergeCell ref="E126:E127"/>
-    <mergeCell ref="F126:F127"/>
-    <mergeCell ref="A131:F131"/>
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="F11:F14"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A44:F44"/>
     <mergeCell ref="A113:F113"/>
     <mergeCell ref="A63:F63"/>
     <mergeCell ref="A69:F69"/>
@@ -45175,18 +45179,14 @@
     <mergeCell ref="E93:E94"/>
     <mergeCell ref="F93:F94"/>
     <mergeCell ref="A102:F102"/>
-    <mergeCell ref="A54:F54"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="E11:E14"/>
-    <mergeCell ref="F11:F14"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A44:F44"/>
+    <mergeCell ref="A142:F142"/>
+    <mergeCell ref="A155:F155"/>
+    <mergeCell ref="E114:E115"/>
+    <mergeCell ref="F114:F115"/>
+    <mergeCell ref="A125:F125"/>
+    <mergeCell ref="E126:E127"/>
+    <mergeCell ref="F126:F127"/>
+    <mergeCell ref="A131:F131"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>